<commit_message>
Aggiunta possibilità di avere etichette in italiano
</commit_message>
<xml_diff>
--- a/data-raw/data_raw.xlsx
+++ b/data-raw/data_raw.xlsx
@@ -5,27 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/ecoservr/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mela\OneDrive - RSE S.p.A\R\miei_pacchetti\ecoservr\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1339" documentId="11_AD4D5CB4E552A5DACE1C64C0901D4AE65BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{353F92F5-3DD7-4380-A03B-0215E75A8A23}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="315" windowWidth="12900" windowHeight="14310" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="540" yWindow="660" windowWidth="12900" windowHeight="14310" firstSheet="6" activeTab="7" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
   </bookViews>
   <sheets>
     <sheet name="maes_corine" sheetId="2" r:id="rId1"/>
     <sheet name="master_table_agr" sheetId="12" r:id="rId2"/>
-    <sheet name="pollination_key" sheetId="14" r:id="rId3"/>
-    <sheet name="eco_con_coeff" sheetId="3" r:id="rId4"/>
-    <sheet name="nuts2_codes" sheetId="9" r:id="rId5"/>
-    <sheet name="pollination_dependence" sheetId="15" r:id="rId6"/>
-    <sheet name="pollination_crops" sheetId="17" r:id="rId7"/>
-    <sheet name="landscape_values" sheetId="16" r:id="rId8"/>
+    <sheet name="crop_names_it_en" sheetId="18" r:id="rId3"/>
+    <sheet name="pollination_key" sheetId="14" r:id="rId4"/>
+    <sheet name="eco_con_coeff" sheetId="3" r:id="rId5"/>
+    <sheet name="nuts2_codes" sheetId="9" r:id="rId6"/>
+    <sheet name="pollination_dependence" sheetId="15" r:id="rId7"/>
+    <sheet name="pollination_crops" sheetId="17" r:id="rId8"/>
+    <sheet name="landscape_values" sheetId="16" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">master_table_agr!$A$1:$J$53</definedName>
-    <definedName name="DatiEsterni_1" localSheetId="4" hidden="1">nuts2_codes!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">master_table_agr!$A$1:$L$53</definedName>
+    <definedName name="DatiEsterni_1" localSheetId="5" hidden="1">nuts2_codes!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="500">
   <si>
     <t>Urban</t>
   </si>
@@ -1460,6 +1461,108 @@
   </si>
   <si>
     <t>all_crops</t>
+  </si>
+  <si>
+    <t>label_en</t>
+  </si>
+  <si>
+    <t>Orzo</t>
+  </si>
+  <si>
+    <t>Agrumi</t>
+  </si>
+  <si>
+    <t>Produzione vegetale</t>
+  </si>
+  <si>
+    <t>Grano duro</t>
+  </si>
+  <si>
+    <t>Mais da foraggio</t>
+  </si>
+  <si>
+    <t>Altre radici foraggere (incluso barbabietola)</t>
+  </si>
+  <si>
+    <t>Frutta fresca</t>
+  </si>
+  <si>
+    <t>Ortaggi</t>
+  </si>
+  <si>
+    <t>Mais da granella</t>
+  </si>
+  <si>
+    <t>Uva</t>
+  </si>
+  <si>
+    <t>Avena</t>
+  </si>
+  <si>
+    <t>Olio di oliva</t>
+  </si>
+  <si>
+    <t>Olive</t>
+  </si>
+  <si>
+    <t>Altri cereali</t>
+  </si>
+  <si>
+    <t>Altre piante da foraggio</t>
+  </si>
+  <si>
+    <t>Altre colture industriali</t>
+  </si>
+  <si>
+    <t>Altre colture oleaginose</t>
+  </si>
+  <si>
+    <t>Piante e fiori</t>
+  </si>
+  <si>
+    <t>Patate</t>
+  </si>
+  <si>
+    <t>Colture proteice</t>
+  </si>
+  <si>
+    <t>Colza</t>
+  </si>
+  <si>
+    <t>Tabacco</t>
+  </si>
+  <si>
+    <t>Riso</t>
+  </si>
+  <si>
+    <t>Grano tenero e farro</t>
+  </si>
+  <si>
+    <t>Soia</t>
+  </si>
+  <si>
+    <t>Barbabietola da zucchero</t>
+  </si>
+  <si>
+    <t>Girasole</t>
+  </si>
+  <si>
+    <t>Frutta tropicale</t>
+  </si>
+  <si>
+    <t>Vino</t>
+  </si>
+  <si>
+    <t>label_it</t>
+  </si>
+  <si>
+    <t>corine3_label_en</t>
+  </si>
+  <si>
+    <t>value_label_en</t>
+  </si>
+  <si>
+    <t>value_label_it</t>
   </si>
 </sst>
 </file>
@@ -1786,443 +1889,563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F990C3D9-B8AC-4A3C-9113-97EA19847D8C}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A4" workbookViewId="1">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>497</v>
       </c>
       <c r="B1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" t="s">
         <v>184</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2">
         <v>111</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C3">
         <v>112</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4">
         <v>121</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5">
         <v>122</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6">
         <v>123</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7">
         <v>124</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8">
         <v>131</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9">
         <v>132</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10">
         <v>133</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11">
         <v>141</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12">
         <v>142</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13">
         <v>211</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>335</v>
+      </c>
+      <c r="C14">
         <v>212</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C15">
         <v>213</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C16">
         <v>221</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>338</v>
+      </c>
+      <c r="C17">
         <v>222</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>339</v>
+      </c>
+      <c r="C18">
         <v>223</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19">
         <v>241</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20">
         <v>242</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21">
         <v>243</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>345</v>
+      </c>
+      <c r="C22">
         <v>244</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="s">
+        <v>352</v>
+      </c>
+      <c r="C23">
         <v>321</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>340</v>
+      </c>
+      <c r="C24">
         <v>231</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="s">
+        <v>353</v>
+      </c>
+      <c r="C25">
         <v>322</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="s">
+        <v>354</v>
+      </c>
+      <c r="C26">
         <v>323</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="s">
+        <v>346</v>
+      </c>
+      <c r="C27">
         <v>311</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28">
         <v>312</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="s">
+        <v>351</v>
+      </c>
+      <c r="C29">
         <v>313</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="s">
+        <v>356</v>
+      </c>
+      <c r="C30">
         <v>324</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="s">
+        <v>358</v>
+      </c>
+      <c r="C31">
         <v>331</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="s">
+        <v>360</v>
+      </c>
+      <c r="C32">
         <v>332</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="s">
+        <v>361</v>
+      </c>
+      <c r="C33">
         <v>333</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="s">
+        <v>362</v>
+      </c>
+      <c r="C34">
         <v>334</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="s">
+        <v>363</v>
+      </c>
+      <c r="C35">
         <v>335</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="s">
+        <v>364</v>
+      </c>
+      <c r="C36">
         <v>411</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="s">
+        <v>366</v>
+      </c>
+      <c r="C37">
         <v>412</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="s">
+        <v>374</v>
+      </c>
+      <c r="C38">
         <v>511</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="s">
+        <v>375</v>
+      </c>
+      <c r="C39">
         <v>512</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2234,1719 +2457,2040 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B7B9A9-54CC-4D8F-A3E8-5153520FA509}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:H53"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>498</v>
       </c>
       <c r="B1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1" t="s">
         <v>150</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>191</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>149</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>186</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>184</v>
       </c>
-      <c r="H1" t="s">
-        <v>222</v>
-      </c>
       <c r="I1" t="s">
+        <v>497</v>
+      </c>
+      <c r="J1" t="s">
+        <v>383</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>192</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>187</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.121</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>211</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>333</v>
+      </c>
+      <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>192</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>187</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.11</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>211</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>333</v>
+      </c>
+      <c r="K3" t="s">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>192</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>187</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.189</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>211</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>333</v>
+      </c>
+      <c r="K4" t="s">
         <v>2</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>477</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>192</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>74</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>187</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.187</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>211</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>333</v>
+      </c>
+      <c r="K5" t="s">
         <v>2</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>477</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>192</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>75</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>187</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.187</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>211</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>333</v>
+      </c>
+      <c r="K6" t="s">
         <v>2</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>475</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>192</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>76</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>187</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.121</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>211</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>333</v>
+      </c>
+      <c r="K7" t="s">
         <v>2</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>163</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>192</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>187</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>9.4E-2</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>211</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>333</v>
+      </c>
+      <c r="K8" t="s">
         <v>2</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>480</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>192</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>70</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>187</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>9.4E-2</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>211</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>18</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>333</v>
+      </c>
+      <c r="K9" t="s">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>480</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>192</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>77</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>187</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>9.4E-2</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>211</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>333</v>
+      </c>
+      <c r="K10" t="s">
         <v>2</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>480</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>192</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>78</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>187</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>9.4E-2</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>211</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>333</v>
+      </c>
+      <c r="K11" t="s">
         <v>2</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>480</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>192</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>187</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>9.4E-2</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>211</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>18</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>333</v>
+      </c>
+      <c r="K12" t="s">
         <v>2</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>489</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>192</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>151</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>187</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>9.4E-2</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>213</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>20</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
+        <v>336</v>
+      </c>
+      <c r="K13" t="s">
         <v>2</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>487</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>192</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>84</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>187</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0.15</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>211</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>18</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
+        <v>333</v>
+      </c>
+      <c r="K14" t="s">
         <v>2</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>493</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>192</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>85</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>187</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>0.20899999999999999</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>211</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
+        <v>333</v>
+      </c>
+      <c r="K15" t="s">
         <v>2</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>491</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>192</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>86</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>187</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>0.155</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>211</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>18</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
+        <v>333</v>
+      </c>
+      <c r="K16" t="s">
         <v>2</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>483</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>192</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>88</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>187</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>0.155</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>211</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>18</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
+        <v>333</v>
+      </c>
+      <c r="K17" t="s">
         <v>2</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>483</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>192</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>89</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>187</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>0.155</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>211</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>18</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
+        <v>333</v>
+      </c>
+      <c r="K18" t="s">
         <v>2</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>483</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>192</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>90</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>187</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>0.155</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>211</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>18</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
+        <v>333</v>
+      </c>
+      <c r="K19" t="s">
         <v>2</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>488</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>192</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>95</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>187</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>0.155</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>211</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>18</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
+        <v>333</v>
+      </c>
+      <c r="K20" t="s">
         <v>2</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>180</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>482</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>192</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>91</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>187</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>0.155</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>211</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>18</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>333</v>
+      </c>
+      <c r="K21" t="s">
         <v>2</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>180</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>482</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>192</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>96</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>187</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>0.155</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>211</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>18</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>333</v>
+      </c>
+      <c r="K22" t="s">
         <v>2</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>180</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>482</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>192</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>97</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>187</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>0.155</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>211</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>18</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
+        <v>333</v>
+      </c>
+      <c r="K23" t="s">
         <v>2</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>180</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>192</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>98</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>187</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>0.155</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>211</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>18</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
+        <v>333</v>
+      </c>
+      <c r="K24" t="s">
         <v>2</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>180</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>482</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>192</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>99</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>187</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>0.155</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>211</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>18</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
+        <v>333</v>
+      </c>
+      <c r="K25" t="s">
         <v>2</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>180</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>482</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>192</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>92</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>187</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>0.155</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>211</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>18</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
+        <v>333</v>
+      </c>
+      <c r="K26" t="s">
         <v>2</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>482</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>192</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>93</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>187</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>0.155</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>211</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>18</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
+        <v>333</v>
+      </c>
+      <c r="K27" t="s">
         <v>2</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>180</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>482</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>192</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>94</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>187</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>0.155</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>211</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>18</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
+        <v>333</v>
+      </c>
+      <c r="K28" t="s">
         <v>2</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>173</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>485</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>192</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>101</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>187</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>211</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>18</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
+        <v>333</v>
+      </c>
+      <c r="K29" t="s">
         <v>2</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
+        <v>492</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>192</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>102</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>187</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>0.13200000000000001</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>211</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>18</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
+        <v>333</v>
+      </c>
+      <c r="K30" t="s">
         <v>2</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
+        <v>486</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>192</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>100</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>187</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>0.19600000000000001</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>211</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>18</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
+        <v>333</v>
+      </c>
+      <c r="K31" t="s">
         <v>2</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>471</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>192</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>82</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>187</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>0.13100000000000001</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>211</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>18</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
+        <v>333</v>
+      </c>
+      <c r="K32" t="s">
         <v>2</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>169</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>472</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>192</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>103</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>187</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>211</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>18</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
+        <v>333</v>
+      </c>
+      <c r="K33" t="s">
         <v>2</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>481</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>192</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>80</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>187</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>231</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>27</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
+        <v>340</v>
+      </c>
+      <c r="K34" t="s">
         <v>28</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
+        <v>481</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>192</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>81</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>187</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>231</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>27</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
+        <v>340</v>
+      </c>
+      <c r="K35" t="s">
         <v>28</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>170</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
+        <v>481</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>192</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>83</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>187</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>231</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>27</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
+        <v>340</v>
+      </c>
+      <c r="K36" t="s">
         <v>28</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
+        <v>474</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>192</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>104</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>188</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>0.155</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>211</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>18</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
+        <v>333</v>
+      </c>
+      <c r="K37" t="s">
         <v>2</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>172</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
+        <v>484</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>192</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>189</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>188</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>0.155</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>211</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>18</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
+        <v>333</v>
+      </c>
+      <c r="K38" t="s">
         <v>2</v>
       </c>
-      <c r="J38">
+      <c r="L38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>177</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
+        <v>473</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>192</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>153</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>188</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>0.155</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>222</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>21</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
+        <v>338</v>
+      </c>
+      <c r="K39" t="s">
         <v>2</v>
       </c>
-      <c r="J39">
+      <c r="L39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>178</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
+        <v>468</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>192</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>154</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>188</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>0.155</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>222</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>21</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
+        <v>338</v>
+      </c>
+      <c r="K40" t="s">
         <v>2</v>
       </c>
-      <c r="J40">
+      <c r="L40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>181</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
+        <v>494</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>192</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>153</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>188</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>0.155</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>222</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>21</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
+        <v>338</v>
+      </c>
+      <c r="K41" t="s">
         <v>2</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>476</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>192</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>155</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>188</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>0.155</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>221</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>3</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
+        <v>337</v>
+      </c>
+      <c r="K42" t="s">
         <v>2</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>157</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
+        <v>479</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>192</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>158</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>188</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>0.155</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>223</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>22</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
+        <v>339</v>
+      </c>
+      <c r="K43" t="s">
         <v>2</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>174</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>495</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>192</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>155</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>188</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>0.155</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>221</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>3</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
+        <v>337</v>
+      </c>
+      <c r="K44" t="s">
         <v>2</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>182</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
+        <v>478</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>192</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>158</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>188</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>0.155</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>223</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>22</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
+        <v>339</v>
+      </c>
+      <c r="K45" t="s">
         <v>2</v>
       </c>
-      <c r="J45">
+      <c r="L45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>175</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
+        <v>469</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>192</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>190</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>188</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>0.155</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>242</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>24</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
+        <v>343</v>
+      </c>
+      <c r="K46" t="s">
         <v>2</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>175</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
+        <v>469</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>192</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>190</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>188</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>0.155</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>243</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>25</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
+        <v>344</v>
+      </c>
+      <c r="K47" t="s">
         <v>2</v>
       </c>
-      <c r="J47">
+      <c r="L47">
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
+        <v>481</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>192</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>80</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>187</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>321</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>183</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
+        <v>352</v>
+      </c>
+      <c r="K48" t="s">
         <v>28</v>
       </c>
-      <c r="J48">
+      <c r="L48">
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
+        <v>481</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>192</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>81</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>187</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>321</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>183</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
+        <v>352</v>
+      </c>
+      <c r="K49" t="s">
         <v>28</v>
       </c>
-      <c r="J49">
+      <c r="L49">
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
+        <v>481</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>192</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>83</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>187</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>321</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>183</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
+        <v>352</v>
+      </c>
+      <c r="K50" t="s">
         <v>28</v>
       </c>
-      <c r="J50">
+      <c r="L50">
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
+        <v>481</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>192</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>80</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>187</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>244</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>26</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
+        <v>345</v>
+      </c>
+      <c r="K51" t="s">
         <v>28</v>
       </c>
-      <c r="J51">
+      <c r="L51">
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
+        <v>481</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>192</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>81</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>187</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>244</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>26</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
+        <v>345</v>
+      </c>
+      <c r="K52" t="s">
         <v>28</v>
       </c>
-      <c r="J52">
+      <c r="L52">
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>481</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>192</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>83</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>187</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>244</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>26</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K53" t="s">
         <v>28</v>
       </c>
-      <c r="J53">
+      <c r="L53">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O4:P25">
-    <sortCondition ref="P4:P25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q4:R25">
+    <sortCondition ref="R4:R25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3954,6 +4498,265 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB3A8D8-4136-4A9C-9FC8-717369D794A3}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" t="s">
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A30">
+    <sortCondition ref="A2:A30"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD69B390-1B27-424D-8426-FF38F0BAA822}">
   <dimension ref="A1:C78"/>
   <sheetViews>
@@ -4834,7 +5637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDA9136-1659-44E3-AC2D-CCA7F1A09F8B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -5030,7 +5833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1051B5AD-1E4A-4C71-BA18-FC1C7B489DA0}">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -5230,7 +6033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9776A4A5-4824-477A-BFF1-37B09D44A215}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -5410,7 +6213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BE4797-CF48-4FDC-89C4-68FFFF555622}">
   <dimension ref="A1:I33"/>
   <sheetViews>
@@ -5963,14 +6766,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285A83FC-93DE-4924-85CE-252C66D09FA8}">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bug in landscape_values_raw
</commit_message>
<xml_diff>
--- a/data-raw/data_raw.xlsx
+++ b/data-raw/data_raw.xlsx
@@ -5,13 +5,13 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mela\OneDrive - RSE S.p.A\R\miei_pacchetti\ecoservr\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/ecoservr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{023C88C8-9C5E-485C-BA46-E380A7FC5548}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="8" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
   </bookViews>
   <sheets>
     <sheet name="maes_corine" sheetId="2" r:id="rId1"/>
@@ -1086,9 +1086,6 @@
     <t>Prati stabili (foraggere permanenti)</t>
   </si>
   <si>
-    <t>Grassland</t>
-  </si>
-  <si>
     <t>Colture temporanee associate a colture permanenti</t>
   </si>
   <si>
@@ -1563,6 +1560,9 @@
   </si>
   <si>
     <t>value_label_it</t>
+  </si>
+  <si>
+    <t>Natural Grasslands</t>
   </si>
 </sst>
 </file>
@@ -1905,10 +1905,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C1" t="s">
         <v>184</v>
@@ -2160,7 +2160,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C19">
         <v>241</v>
@@ -2174,7 +2174,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C20">
         <v>242</v>
@@ -2188,7 +2188,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C21">
         <v>243</v>
@@ -2202,7 +2202,7 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C22">
         <v>244</v>
@@ -2216,7 +2216,7 @@
         <v>183</v>
       </c>
       <c r="B23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C23">
         <v>321</v>
@@ -2244,7 +2244,7 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C25">
         <v>322</v>
@@ -2258,7 +2258,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C26">
         <v>323</v>
@@ -2272,7 +2272,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C27">
         <v>311</v>
@@ -2286,7 +2286,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C28">
         <v>312</v>
@@ -2300,7 +2300,7 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C29">
         <v>313</v>
@@ -2314,7 +2314,7 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C30">
         <v>324</v>
@@ -2328,7 +2328,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C31">
         <v>331</v>
@@ -2342,7 +2342,7 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C32">
         <v>332</v>
@@ -2356,7 +2356,7 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C33">
         <v>333</v>
@@ -2370,7 +2370,7 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C34">
         <v>334</v>
@@ -2384,7 +2384,7 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C35">
         <v>335</v>
@@ -2398,7 +2398,7 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C36">
         <v>411</v>
@@ -2412,7 +2412,7 @@
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C37">
         <v>412</v>
@@ -2426,7 +2426,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C38">
         <v>511</v>
@@ -2440,7 +2440,7 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C39">
         <v>512</v>
@@ -2462,7 +2462,7 @@
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:H53"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2476,10 +2476,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" t="s">
         <v>498</v>
-      </c>
-      <c r="B1" t="s">
-        <v>499</v>
       </c>
       <c r="C1" t="s">
         <v>150</v>
@@ -2500,10 +2500,10 @@
         <v>184</v>
       </c>
       <c r="I1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -2517,7 +2517,7 @@
         <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>193</v>
@@ -2555,7 +2555,7 @@
         <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>194</v>
@@ -2593,7 +2593,7 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>195</v>
@@ -2631,7 +2631,7 @@
         <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>196</v>
@@ -2669,7 +2669,7 @@
         <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>196</v>
@@ -2707,7 +2707,7 @@
         <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>197</v>
@@ -2745,7 +2745,7 @@
         <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>198</v>
@@ -2783,7 +2783,7 @@
         <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>198</v>
@@ -2821,7 +2821,7 @@
         <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>198</v>
@@ -2859,7 +2859,7 @@
         <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>198</v>
@@ -2897,7 +2897,7 @@
         <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>198</v>
@@ -2935,7 +2935,7 @@
         <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>199</v>
@@ -2973,7 +2973,7 @@
         <v>164</v>
       </c>
       <c r="B14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>200</v>
@@ -3011,7 +3011,7 @@
         <v>165</v>
       </c>
       <c r="B15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>201</v>
@@ -3049,7 +3049,7 @@
         <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>202</v>
@@ -3087,7 +3087,7 @@
         <v>179</v>
       </c>
       <c r="B17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>203</v>
@@ -3125,7 +3125,7 @@
         <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>203</v>
@@ -3163,7 +3163,7 @@
         <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>203</v>
@@ -3201,7 +3201,7 @@
         <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>204</v>
@@ -3239,7 +3239,7 @@
         <v>180</v>
       </c>
       <c r="B21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>205</v>
@@ -3277,7 +3277,7 @@
         <v>180</v>
       </c>
       <c r="B22" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>205</v>
@@ -3315,7 +3315,7 @@
         <v>180</v>
       </c>
       <c r="B23" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>205</v>
@@ -3353,7 +3353,7 @@
         <v>180</v>
       </c>
       <c r="B24" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>205</v>
@@ -3391,7 +3391,7 @@
         <v>180</v>
       </c>
       <c r="B25" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>205</v>
@@ -3429,7 +3429,7 @@
         <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>205</v>
@@ -3467,7 +3467,7 @@
         <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>205</v>
@@ -3505,7 +3505,7 @@
         <v>180</v>
       </c>
       <c r="B28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>205</v>
@@ -3543,7 +3543,7 @@
         <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>206</v>
@@ -3581,7 +3581,7 @@
         <v>167</v>
       </c>
       <c r="B30" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>207</v>
@@ -3619,7 +3619,7 @@
         <v>176</v>
       </c>
       <c r="B31" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>208</v>
@@ -3657,7 +3657,7 @@
         <v>168</v>
       </c>
       <c r="B32" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>209</v>
@@ -3695,7 +3695,7 @@
         <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>210</v>
@@ -3733,7 +3733,7 @@
         <v>170</v>
       </c>
       <c r="B34" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>211</v>
@@ -3771,7 +3771,7 @@
         <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>211</v>
@@ -3809,7 +3809,7 @@
         <v>170</v>
       </c>
       <c r="B36" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>211</v>
@@ -3847,7 +3847,7 @@
         <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>212</v>
@@ -3885,7 +3885,7 @@
         <v>172</v>
       </c>
       <c r="B38" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>213</v>
@@ -3923,7 +3923,7 @@
         <v>177</v>
       </c>
       <c r="B39" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>214</v>
@@ -3961,7 +3961,7 @@
         <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>221</v>
@@ -3999,7 +3999,7 @@
         <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>215</v>
@@ -4037,7 +4037,7 @@
         <v>156</v>
       </c>
       <c r="B42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>216</v>
@@ -4075,7 +4075,7 @@
         <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>217</v>
@@ -4113,7 +4113,7 @@
         <v>174</v>
       </c>
       <c r="B44" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>218</v>
@@ -4151,7 +4151,7 @@
         <v>182</v>
       </c>
       <c r="B45" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>219</v>
@@ -4189,7 +4189,7 @@
         <v>175</v>
       </c>
       <c r="B46" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>220</v>
@@ -4213,7 +4213,7 @@
         <v>24</v>
       </c>
       <c r="J46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K46" t="s">
         <v>2</v>
@@ -4227,7 +4227,7 @@
         <v>175</v>
       </c>
       <c r="B47" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>220</v>
@@ -4251,7 +4251,7 @@
         <v>25</v>
       </c>
       <c r="J47" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K47" t="s">
         <v>2</v>
@@ -4265,7 +4265,7 @@
         <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>211</v>
@@ -4289,7 +4289,7 @@
         <v>183</v>
       </c>
       <c r="J48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K48" t="s">
         <v>28</v>
@@ -4303,7 +4303,7 @@
         <v>170</v>
       </c>
       <c r="B49" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>211</v>
@@ -4327,7 +4327,7 @@
         <v>183</v>
       </c>
       <c r="J49" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K49" t="s">
         <v>28</v>
@@ -4341,7 +4341,7 @@
         <v>170</v>
       </c>
       <c r="B50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>211</v>
@@ -4365,7 +4365,7 @@
         <v>183</v>
       </c>
       <c r="J50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K50" t="s">
         <v>28</v>
@@ -4379,7 +4379,7 @@
         <v>170</v>
       </c>
       <c r="B51" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>211</v>
@@ -4403,7 +4403,7 @@
         <v>26</v>
       </c>
       <c r="J51" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K51" t="s">
         <v>28</v>
@@ -4417,7 +4417,7 @@
         <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>211</v>
@@ -4441,7 +4441,7 @@
         <v>26</v>
       </c>
       <c r="J52" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K52" t="s">
         <v>28</v>
@@ -4455,7 +4455,7 @@
         <v>170</v>
       </c>
       <c r="B53" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>211</v>
@@ -4479,7 +4479,7 @@
         <v>26</v>
       </c>
       <c r="J53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K53" t="s">
         <v>28</v>
@@ -4510,10 +4510,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4529,7 +4529,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4537,7 +4537,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4545,7 +4545,7 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4553,7 +4553,7 @@
         <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4561,7 +4561,7 @@
         <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
         <v>162</v>
       </c>
       <c r="B10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4593,7 +4593,7 @@
         <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4601,7 +4601,7 @@
         <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4609,7 +4609,7 @@
         <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4617,7 +4617,7 @@
         <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4625,7 +4625,7 @@
         <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4633,7 +4633,7 @@
         <v>170</v>
       </c>
       <c r="B16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>180</v>
       </c>
       <c r="B17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -4649,7 +4649,7 @@
         <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4657,7 +4657,7 @@
         <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
         <v>173</v>
       </c>
       <c r="B20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>176</v>
       </c>
       <c r="B21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4681,7 +4681,7 @@
         <v>164</v>
       </c>
       <c r="B22" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4689,7 +4689,7 @@
         <v>166</v>
       </c>
       <c r="B23" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -4697,7 +4697,7 @@
         <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -4705,7 +4705,7 @@
         <v>160</v>
       </c>
       <c r="B25" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4713,7 +4713,7 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -4721,7 +4721,7 @@
         <v>167</v>
       </c>
       <c r="B27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
         <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -4737,7 +4737,7 @@
         <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -4745,7 +4745,7 @@
         <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -6051,10 +6051,10 @@
         <v>311</v>
       </c>
       <c r="B1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C1" t="s">
         <v>463</v>
-      </c>
-      <c r="C1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6202,7 +6202,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C15">
         <v>0.10447198275862069</v>
@@ -6231,10 +6231,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C1" t="s">
         <v>149</v>
@@ -6254,13 +6254,13 @@
         <v>244</v>
       </c>
       <c r="C2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -6275,13 +6275,13 @@
         <v>245</v>
       </c>
       <c r="C3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D3" t="s">
         <v>246</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -6296,7 +6296,7 @@
         <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -6312,7 +6312,7 @@
         <v>237</v>
       </c>
       <c r="C5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6323,7 +6323,7 @@
         <v>240</v>
       </c>
       <c r="C6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6334,13 +6334,13 @@
         <v>241</v>
       </c>
       <c r="C7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E7" t="s">
         <v>436</v>
-      </c>
-      <c r="E7" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6351,13 +6351,13 @@
         <v>229</v>
       </c>
       <c r="C8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D8" t="s">
+        <v>437</v>
+      </c>
+      <c r="E8" t="s">
         <v>438</v>
-      </c>
-      <c r="E8" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6365,28 +6365,28 @@
         <v>229</v>
       </c>
       <c r="B9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C9" t="s">
         <v>391</v>
-      </c>
-      <c r="C9" t="s">
-        <v>392</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B10" t="s">
         <v>301</v>
       </c>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D10" t="s">
+        <v>439</v>
+      </c>
+      <c r="E10" t="s">
         <v>440</v>
-      </c>
-      <c r="E10" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6397,13 +6397,13 @@
         <v>223</v>
       </c>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D11" t="s">
+        <v>441</v>
+      </c>
+      <c r="E11" t="s">
         <v>442</v>
-      </c>
-      <c r="E11" t="s">
-        <v>443</v>
       </c>
       <c r="H11" t="s">
         <v>233</v>
@@ -6417,19 +6417,19 @@
         <v>255</v>
       </c>
       <c r="B12" t="s">
+        <v>394</v>
+      </c>
+      <c r="C12" t="s">
         <v>395</v>
-      </c>
-      <c r="C12" t="s">
-        <v>396</v>
       </c>
       <c r="D12" t="s">
         <v>251</v>
       </c>
       <c r="E12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I12">
         <v>80434.850000000006</v>
@@ -6443,13 +6443,13 @@
         <v>253</v>
       </c>
       <c r="C13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D13" t="s">
         <v>254</v>
       </c>
       <c r="E13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H13" t="s">
         <v>246</v>
@@ -6460,16 +6460,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B14" t="s">
         <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I14">
         <v>339073.1</v>
@@ -6483,7 +6483,7 @@
         <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H15" t="s">
         <v>251</v>
@@ -6500,7 +6500,7 @@
         <v>242</v>
       </c>
       <c r="C16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H16" t="s">
         <v>254</v>
@@ -6511,19 +6511,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B17" t="s">
         <v>294</v>
       </c>
       <c r="C17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I17">
         <f>+I11-SUM(I12:I16)</f>
@@ -6538,92 +6538,92 @@
         <v>230</v>
       </c>
       <c r="C18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B19" t="s">
         <v>292</v>
       </c>
       <c r="C19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B20" t="s">
+        <v>451</v>
+      </c>
+      <c r="C20" t="s">
         <v>452</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>454</v>
+      </c>
+      <c r="E20" t="s">
         <v>453</v>
-      </c>
-      <c r="D20" t="s">
-        <v>455</v>
-      </c>
-      <c r="E20" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C21" t="s">
         <v>404</v>
-      </c>
-      <c r="C21" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B22" t="s">
         <v>298</v>
       </c>
       <c r="C22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D22" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B23" t="s">
         <v>297</v>
       </c>
       <c r="C23" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D23" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E23" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6634,35 +6634,35 @@
         <v>310</v>
       </c>
       <c r="C24" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>408</v>
+      </c>
+      <c r="B25" t="s">
+        <v>408</v>
+      </c>
+      <c r="C25" t="s">
         <v>409</v>
-      </c>
-      <c r="B25" t="s">
-        <v>409</v>
-      </c>
-      <c r="C25" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B26" t="s">
         <v>307</v>
       </c>
       <c r="C26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E26" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6673,7 +6673,7 @@
         <v>275</v>
       </c>
       <c r="C27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -6684,13 +6684,13 @@
         <v>278</v>
       </c>
       <c r="C28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D28" t="s">
         <v>278</v>
       </c>
       <c r="E28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6701,13 +6701,13 @@
         <v>276</v>
       </c>
       <c r="C29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D29" t="s">
         <v>276</v>
       </c>
       <c r="E29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -6718,13 +6718,13 @@
         <v>300</v>
       </c>
       <c r="C30" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D30" t="s">
         <v>299</v>
       </c>
       <c r="E30" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -6735,7 +6735,7 @@
         <v>315</v>
       </c>
       <c r="C31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -6746,18 +6746,18 @@
         <v>314</v>
       </c>
       <c r="C32" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B33" t="s">
+        <v>417</v>
+      </c>
+      <c r="C33" t="s">
         <v>418</v>
-      </c>
-      <c r="C33" t="s">
-        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -6773,8 +6773,8 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6787,7 +6787,7 @@
         <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -7180,7 +7180,7 @@
         <v>340</v>
       </c>
       <c r="D19" t="s">
-        <v>341</v>
+        <v>28</v>
       </c>
       <c r="E19">
         <v>331</v>
@@ -7206,7 +7206,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
@@ -7235,7 +7235,7 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
@@ -7264,7 +7264,7 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
@@ -7293,7 +7293,7 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D23" t="s">
         <v>2</v>
@@ -7322,7 +7322,7 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -7331,16 +7331,16 @@
         <v>254</v>
       </c>
       <c r="F24" t="s">
+        <v>346</v>
+      </c>
+      <c r="G24" t="s">
         <v>347</v>
-      </c>
-      <c r="G24" t="s">
-        <v>348</v>
       </c>
       <c r="H24">
         <v>2007</v>
       </c>
       <c r="I24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -7351,7 +7351,7 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -7360,16 +7360,16 @@
         <v>254</v>
       </c>
       <c r="F25" t="s">
+        <v>346</v>
+      </c>
+      <c r="G25" t="s">
         <v>347</v>
-      </c>
-      <c r="G25" t="s">
-        <v>348</v>
       </c>
       <c r="H25">
         <v>2007</v>
       </c>
       <c r="I25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -7380,7 +7380,7 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -7389,16 +7389,16 @@
         <v>254</v>
       </c>
       <c r="F26" t="s">
+        <v>346</v>
+      </c>
+      <c r="G26" t="s">
         <v>347</v>
-      </c>
-      <c r="G26" t="s">
-        <v>348</v>
       </c>
       <c r="H26">
         <v>2007</v>
       </c>
       <c r="I26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -7406,13 +7406,13 @@
         <v>321</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>499</v>
       </c>
       <c r="C27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D27" t="s">
-        <v>341</v>
+        <v>28</v>
       </c>
       <c r="E27">
         <v>331</v>
@@ -7438,7 +7438,7 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -7447,16 +7447,16 @@
         <v>254</v>
       </c>
       <c r="F28" t="s">
+        <v>346</v>
+      </c>
+      <c r="G28" t="s">
         <v>347</v>
-      </c>
-      <c r="G28" t="s">
-        <v>348</v>
       </c>
       <c r="H28">
         <v>2007</v>
       </c>
       <c r="I28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -7467,7 +7467,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -7476,16 +7476,16 @@
         <v>254</v>
       </c>
       <c r="F29" t="s">
+        <v>346</v>
+      </c>
+      <c r="G29" t="s">
         <v>347</v>
-      </c>
-      <c r="G29" t="s">
-        <v>348</v>
       </c>
       <c r="H29">
         <v>2007</v>
       </c>
       <c r="I29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -7493,10 +7493,10 @@
         <v>324</v>
       </c>
       <c r="B30" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" t="s">
         <v>355</v>
-      </c>
-      <c r="C30" t="s">
-        <v>356</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -7505,16 +7505,16 @@
         <v>254</v>
       </c>
       <c r="F30" t="s">
+        <v>346</v>
+      </c>
+      <c r="G30" t="s">
         <v>347</v>
-      </c>
-      <c r="G30" t="s">
-        <v>348</v>
       </c>
       <c r="H30">
         <v>2007</v>
       </c>
       <c r="I30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -7522,10 +7522,10 @@
         <v>331</v>
       </c>
       <c r="B31" t="s">
+        <v>356</v>
+      </c>
+      <c r="C31" t="s">
         <v>357</v>
-      </c>
-      <c r="C31" t="s">
-        <v>358</v>
       </c>
       <c r="D31" t="s">
         <v>37</v>
@@ -7539,10 +7539,10 @@
         <v>332</v>
       </c>
       <c r="B32" t="s">
+        <v>358</v>
+      </c>
+      <c r="C32" t="s">
         <v>359</v>
-      </c>
-      <c r="C32" t="s">
-        <v>360</v>
       </c>
       <c r="D32" t="s">
         <v>37</v>
@@ -7559,7 +7559,7 @@
         <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D33" t="s">
         <v>37</v>
@@ -7576,7 +7576,7 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D34" t="s">
         <v>37</v>
@@ -7593,7 +7593,7 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -7610,7 +7610,7 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D36" t="s">
         <v>42</v>
@@ -7624,10 +7624,10 @@
         <v>412</v>
       </c>
       <c r="B37" t="s">
+        <v>364</v>
+      </c>
+      <c r="C37" t="s">
         <v>365</v>
-      </c>
-      <c r="C37" t="s">
-        <v>366</v>
       </c>
       <c r="D37" t="s">
         <v>42</v>
@@ -7641,13 +7641,13 @@
         <v>421</v>
       </c>
       <c r="B38" t="s">
+        <v>366</v>
+      </c>
+      <c r="C38" t="s">
         <v>367</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>368</v>
-      </c>
-      <c r="D38" t="s">
-        <v>369</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -7658,13 +7658,13 @@
         <v>422</v>
       </c>
       <c r="B39" t="s">
+        <v>369</v>
+      </c>
+      <c r="C39" t="s">
         <v>370</v>
       </c>
-      <c r="C39" t="s">
-        <v>371</v>
-      </c>
       <c r="D39" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -7675,13 +7675,13 @@
         <v>423</v>
       </c>
       <c r="B40" t="s">
+        <v>371</v>
+      </c>
+      <c r="C40" t="s">
         <v>372</v>
       </c>
-      <c r="C40" t="s">
-        <v>373</v>
-      </c>
       <c r="D40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -7695,7 +7695,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D41" t="s">
         <v>45</v>
@@ -7712,7 +7712,7 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D42" t="s">
         <v>45</v>
@@ -7726,13 +7726,13 @@
         <v>521</v>
       </c>
       <c r="B43" t="s">
+        <v>375</v>
+      </c>
+      <c r="C43" t="s">
         <v>376</v>
       </c>
-      <c r="C43" t="s">
-        <v>377</v>
-      </c>
       <c r="D43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -7743,13 +7743,13 @@
         <v>522</v>
       </c>
       <c r="B44" t="s">
+        <v>377</v>
+      </c>
+      <c r="C44" t="s">
         <v>378</v>
       </c>
-      <c r="C44" t="s">
-        <v>379</v>
-      </c>
       <c r="D44" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -7760,13 +7760,13 @@
         <v>523</v>
       </c>
       <c r="B45" t="s">
+        <v>379</v>
+      </c>
+      <c r="C45" t="s">
         <v>380</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>381</v>
-      </c>
-      <c r="D45" t="s">
-        <v>382</v>
       </c>
       <c r="E45">
         <v>0</v>

</xml_diff>

<commit_message>
Included option to get ecosystem service values calculated for ecosystems and not corine codes.
</commit_message>
<xml_diff>
--- a/data-raw/data_raw.xlsx
+++ b/data-raw/data_raw.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/ecoservr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{023C88C8-9C5E-485C-BA46-E380A7FC5548}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324B3049-B190-463A-B298-22D2F160A80C}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="8" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="8" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
   </bookViews>
   <sheets>
     <sheet name="maes_corine" sheetId="2" r:id="rId1"/>
@@ -1891,8 +1890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F990C3D9-B8AC-4A3C-9113-97EA19847D8C}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView topLeftCell="A4" workbookViewId="1">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2459,10 +2457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B7B9A9-54CC-4D8F-A3E8-5153520FA509}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H53"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2472,6 +2467,7 @@
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="84.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4406,7 +4402,7 @@
         <v>344</v>
       </c>
       <c r="K51" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L51">
         <v>0.5</v>
@@ -4444,7 +4440,7 @@
         <v>344</v>
       </c>
       <c r="K52" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L52">
         <v>0.5</v>
@@ -4482,13 +4478,14 @@
         <v>344</v>
       </c>
       <c r="K53" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L53">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L53" xr:uid="{B3B7B9A9-54CC-4D8F-A3E8-5153520FA509}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q4:R25">
     <sortCondition ref="R4:R25"/>
   </sortState>
@@ -4501,8 +4498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB3A8D8-4136-4A9C-9FC8-717369D794A3}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4760,10 +4756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD69B390-1B27-424D-8426-FF38F0BAA822}">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C78"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5641,10 +5634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDA9136-1659-44E3-AC2D-CCA7F1A09F8B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C16"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5837,10 +5827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1051B5AD-1E4A-4C71-BA18-FC1C7B489DA0}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6038,9 +6025,6 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6217,10 +6201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BE4797-CF48-4FDC-89C4-68FFFF555622}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6771,9 +6752,6 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Aggiornata funzione compute_agr_value, adesso accetta che il codice corine 212
</commit_message>
<xml_diff>
--- a/data-raw/data_raw.xlsx
+++ b/data-raw/data_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/ecoservr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324B3049-B190-463A-B298-22D2F160A80C}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{7DB053A2-2930-4A76-8476-84542FB883CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF858ACA-AC95-48E5-AC92-CBAFB9A18586}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="8" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
+    <workbookView xWindow="0" yWindow="1245" windowWidth="27000" windowHeight="14235" activeTab="1" xr2:uid="{72F8A742-DF1C-40B1-BF14-E9ADE65D289C}"/>
   </bookViews>
   <sheets>
     <sheet name="maes_corine" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="landscape_values" sheetId="16" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">master_table_agr!$A$1:$L$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">master_table_agr!$A$1:$L$54</definedName>
     <definedName name="DatiEsterni_1" localSheetId="5" hidden="1">nuts2_codes!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="500">
   <si>
     <t>Urban</t>
   </si>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F990C3D9-B8AC-4A3C-9113-97EA19847D8C}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,10 +2455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3B7B9A9-54CC-4D8F-A3E8-5153520FA509}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,34 +2928,34 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
         <v>192</v>
       </c>
       <c r="E13" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
         <v>187</v>
       </c>
       <c r="G13">
-        <v>9.4E-2</v>
+        <v>0.15</v>
       </c>
       <c r="H13">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K13" t="s">
         <v>2</v>
@@ -2966,25 +2966,25 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D14" t="s">
         <v>192</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
         <v>187</v>
       </c>
       <c r="G14">
-        <v>0.15</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="H14">
         <v>211</v>
@@ -3004,25 +3004,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D15" t="s">
         <v>192</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
         <v>187</v>
       </c>
       <c r="G15">
-        <v>0.20899999999999999</v>
+        <v>0.155</v>
       </c>
       <c r="H15">
         <v>211</v>
@@ -3042,19 +3042,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
       <c r="B16" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D16" t="s">
         <v>192</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
         <v>187</v>
@@ -3092,7 +3092,7 @@
         <v>192</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
         <v>187</v>
@@ -3130,7 +3130,7 @@
         <v>192</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
         <v>187</v>
@@ -3156,19 +3156,19 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D19" t="s">
         <v>192</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
         <v>187</v>
@@ -3194,19 +3194,19 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D20" t="s">
         <v>192</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
         <v>187</v>
@@ -3244,7 +3244,7 @@
         <v>192</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s">
         <v>187</v>
@@ -3282,7 +3282,7 @@
         <v>192</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F22" t="s">
         <v>187</v>
@@ -3320,7 +3320,7 @@
         <v>192</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
         <v>187</v>
@@ -3358,7 +3358,7 @@
         <v>192</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F24" t="s">
         <v>187</v>
@@ -3396,7 +3396,7 @@
         <v>192</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F25" t="s">
         <v>187</v>
@@ -3434,7 +3434,7 @@
         <v>192</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
         <v>187</v>
@@ -3472,7 +3472,7 @@
         <v>192</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F27" t="s">
         <v>187</v>
@@ -3498,25 +3498,25 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D28" t="s">
         <v>192</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F28" t="s">
         <v>187</v>
       </c>
       <c r="G28">
-        <v>0.155</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="H28">
         <v>211</v>
@@ -3536,25 +3536,25 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B29" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D29" t="s">
         <v>192</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F29" t="s">
         <v>187</v>
       </c>
       <c r="G29">
-        <v>8.7999999999999995E-2</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="H29">
         <v>211</v>
@@ -3574,25 +3574,25 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D30" t="s">
         <v>192</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F30" t="s">
         <v>187</v>
       </c>
       <c r="G30">
-        <v>0.13200000000000001</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="H30">
         <v>211</v>
@@ -3612,25 +3612,25 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D31" t="s">
         <v>192</v>
       </c>
       <c r="E31" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
         <v>187</v>
       </c>
       <c r="G31">
-        <v>0.19600000000000001</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="H31">
         <v>211</v>
@@ -3650,25 +3650,25 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D32" t="s">
         <v>192</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F32" t="s">
         <v>187</v>
       </c>
       <c r="G32">
-        <v>0.13100000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H32">
         <v>211</v>
@@ -3688,25 +3688,25 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D33" t="s">
         <v>192</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G33">
-        <v>0.28999999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="H33">
         <v>211</v>
@@ -3726,37 +3726,37 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B34" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D34" t="s">
         <v>192</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
       <c r="F34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G34">
-        <v>0.28999999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="H34">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="I34" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J34" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="K34" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L34">
         <v>1</v>
@@ -3764,37 +3764,37 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
         <v>192</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="F35" t="s">
         <v>187</v>
       </c>
       <c r="G35">
-        <v>0.28999999999999998</v>
+        <v>9.4E-2</v>
       </c>
       <c r="H35">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="I35" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="J35" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="K35" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L35">
         <v>1</v>
@@ -3802,37 +3802,37 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B36" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D36" t="s">
         <v>192</v>
       </c>
       <c r="E36" t="s">
-        <v>83</v>
+        <v>155</v>
       </c>
       <c r="F36" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G36">
-        <v>0.28999999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="H36">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="I36" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="J36" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="K36" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L36">
         <v>1</v>
@@ -3840,19 +3840,19 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>473</v>
+        <v>494</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="D37" t="s">
         <v>192</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="F37" t="s">
         <v>188</v>
@@ -3861,13 +3861,13 @@
         <v>0.155</v>
       </c>
       <c r="H37">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="I37" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="J37" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="K37" t="s">
         <v>2</v>
@@ -3878,19 +3878,19 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D38" t="s">
         <v>192</v>
       </c>
       <c r="E38" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="F38" t="s">
         <v>188</v>
@@ -3899,13 +3899,13 @@
         <v>0.155</v>
       </c>
       <c r="H38">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="I38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J38" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="K38" t="s">
         <v>2</v>
@@ -3916,19 +3916,19 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B39" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D39" t="s">
         <v>192</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F39" t="s">
         <v>188</v>
@@ -3954,19 +3954,19 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B40" t="s">
-        <v>467</v>
+        <v>493</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D40" t="s">
         <v>192</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F40" t="s">
         <v>188</v>
@@ -3992,19 +3992,19 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D41" t="s">
         <v>192</v>
       </c>
       <c r="E41" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="F41" t="s">
         <v>188</v>
@@ -4013,13 +4013,13 @@
         <v>0.155</v>
       </c>
       <c r="H41">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I41" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J41" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K41" t="s">
         <v>2</v>
@@ -4030,19 +4030,19 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="B42" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D42" t="s">
         <v>192</v>
       </c>
       <c r="E42" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F42" t="s">
         <v>188</v>
@@ -4051,13 +4051,13 @@
         <v>0.155</v>
       </c>
       <c r="H42">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I42" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="J42" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="K42" t="s">
         <v>2</v>
@@ -4068,37 +4068,37 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="B43" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D43" t="s">
         <v>192</v>
       </c>
       <c r="E43" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="F43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G43">
-        <v>0.155</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H43">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I43" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="J43" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K43" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -4106,37 +4106,37 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B44" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D44" t="s">
         <v>192</v>
       </c>
       <c r="E44" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="F44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G44">
-        <v>0.155</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H44">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="I44" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="J44" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="K44" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L44">
         <v>1</v>
@@ -4144,37 +4144,37 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B45" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D45" t="s">
         <v>192</v>
       </c>
       <c r="E45" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="F45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G45">
-        <v>0.155</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H45">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I45" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="J45" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K45" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L45">
         <v>1</v>
@@ -4203,13 +4203,13 @@
         <v>0.155</v>
       </c>
       <c r="H46">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K46" t="s">
         <v>2</v>
@@ -4241,13 +4241,13 @@
         <v>0.155</v>
       </c>
       <c r="H47">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K47" t="s">
         <v>2</v>
@@ -4258,37 +4258,37 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B48" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D48" t="s">
         <v>192</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="F48" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G48">
-        <v>0.28999999999999998</v>
+        <v>0.155</v>
       </c>
       <c r="H48">
-        <v>321</v>
+        <v>243</v>
       </c>
       <c r="I48" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="J48" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="K48" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L48">
         <v>0.5</v>
@@ -4308,7 +4308,7 @@
         <v>192</v>
       </c>
       <c r="E49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F49" t="s">
         <v>187</v>
@@ -4317,16 +4317,16 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H49">
-        <v>321</v>
+        <v>244</v>
       </c>
       <c r="I49" t="s">
-        <v>183</v>
+        <v>26</v>
       </c>
       <c r="J49" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="K49" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L49">
         <v>0.5</v>
@@ -4346,7 +4346,7 @@
         <v>192</v>
       </c>
       <c r="E50" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F50" t="s">
         <v>187</v>
@@ -4355,16 +4355,16 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H50">
-        <v>321</v>
+        <v>244</v>
       </c>
       <c r="I50" t="s">
-        <v>183</v>
+        <v>26</v>
       </c>
       <c r="J50" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="K50" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L50">
         <v>0.5</v>
@@ -4384,7 +4384,7 @@
         <v>192</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F51" t="s">
         <v>187</v>
@@ -4422,7 +4422,7 @@
         <v>192</v>
       </c>
       <c r="E52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F52" t="s">
         <v>187</v>
@@ -4431,16 +4431,16 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H52">
-        <v>244</v>
+        <v>321</v>
       </c>
       <c r="I52" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="J52" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="K52" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L52">
         <v>0.5</v>
@@ -4460,7 +4460,7 @@
         <v>192</v>
       </c>
       <c r="E53" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F53" t="s">
         <v>187</v>
@@ -4469,25 +4469,1316 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H53">
-        <v>244</v>
+        <v>321</v>
       </c>
       <c r="I53" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="J53" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="K53" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="L53">
         <v>0.5</v>
       </c>
     </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" t="s">
+        <v>480</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H54">
+        <v>321</v>
+      </c>
+      <c r="I54" t="s">
+        <v>183</v>
+      </c>
+      <c r="J54" t="s">
+        <v>351</v>
+      </c>
+      <c r="K54" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" t="s">
+        <v>489</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D55" t="s">
+        <v>192</v>
+      </c>
+      <c r="E55" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" t="s">
+        <v>187</v>
+      </c>
+      <c r="G55">
+        <v>0.121</v>
+      </c>
+      <c r="H55">
+        <v>212</v>
+      </c>
+      <c r="I55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" t="s">
+        <v>335</v>
+      </c>
+      <c r="K55" t="s">
+        <v>2</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>469</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D56" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" t="s">
+        <v>68</v>
+      </c>
+      <c r="F56" t="s">
+        <v>187</v>
+      </c>
+      <c r="G56">
+        <v>0.11</v>
+      </c>
+      <c r="H56">
+        <v>212</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" t="s">
+        <v>335</v>
+      </c>
+      <c r="K56" t="s">
+        <v>2</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>466</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" t="s">
+        <v>72</v>
+      </c>
+      <c r="F57" t="s">
+        <v>187</v>
+      </c>
+      <c r="G57">
+        <v>0.189</v>
+      </c>
+      <c r="H57">
+        <v>212</v>
+      </c>
+      <c r="I57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J57" t="s">
+        <v>335</v>
+      </c>
+      <c r="K57" t="s">
+        <v>2</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" t="s">
+        <v>476</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" t="s">
+        <v>192</v>
+      </c>
+      <c r="E58" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" t="s">
+        <v>187</v>
+      </c>
+      <c r="G58">
+        <v>0.187</v>
+      </c>
+      <c r="H58">
+        <v>212</v>
+      </c>
+      <c r="I58" t="s">
+        <v>19</v>
+      </c>
+      <c r="J58" t="s">
+        <v>335</v>
+      </c>
+      <c r="K58" t="s">
+        <v>2</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" t="s">
+        <v>476</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F59" t="s">
+        <v>187</v>
+      </c>
+      <c r="G59">
+        <v>0.187</v>
+      </c>
+      <c r="H59">
+        <v>212</v>
+      </c>
+      <c r="I59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59" t="s">
+        <v>335</v>
+      </c>
+      <c r="K59" t="s">
+        <v>2</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" t="s">
+        <v>474</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D60" t="s">
+        <v>192</v>
+      </c>
+      <c r="E60" t="s">
+        <v>76</v>
+      </c>
+      <c r="F60" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60">
+        <v>0.121</v>
+      </c>
+      <c r="H60">
+        <v>212</v>
+      </c>
+      <c r="I60" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60" t="s">
+        <v>335</v>
+      </c>
+      <c r="K60" t="s">
+        <v>2</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" t="s">
+        <v>479</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61" t="s">
+        <v>192</v>
+      </c>
+      <c r="E61" t="s">
+        <v>71</v>
+      </c>
+      <c r="F61" t="s">
+        <v>187</v>
+      </c>
+      <c r="G61">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H61">
+        <v>212</v>
+      </c>
+      <c r="I61" t="s">
+        <v>19</v>
+      </c>
+      <c r="J61" t="s">
+        <v>335</v>
+      </c>
+      <c r="K61" t="s">
+        <v>2</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" t="s">
+        <v>479</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D62" t="s">
+        <v>192</v>
+      </c>
+      <c r="E62" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" t="s">
+        <v>187</v>
+      </c>
+      <c r="G62">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H62">
+        <v>212</v>
+      </c>
+      <c r="I62" t="s">
+        <v>19</v>
+      </c>
+      <c r="J62" t="s">
+        <v>335</v>
+      </c>
+      <c r="K62" t="s">
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63" t="s">
+        <v>479</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63" t="s">
+        <v>192</v>
+      </c>
+      <c r="E63" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" t="s">
+        <v>187</v>
+      </c>
+      <c r="G63">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H63">
+        <v>212</v>
+      </c>
+      <c r="I63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J63" t="s">
+        <v>335</v>
+      </c>
+      <c r="K63" t="s">
+        <v>2</v>
+      </c>
+      <c r="L63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" t="s">
+        <v>479</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D64" t="s">
+        <v>192</v>
+      </c>
+      <c r="E64" t="s">
+        <v>78</v>
+      </c>
+      <c r="F64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G64">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H64">
+        <v>212</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J64" t="s">
+        <v>335</v>
+      </c>
+      <c r="K64" t="s">
+        <v>2</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" t="s">
+        <v>479</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" t="s">
+        <v>79</v>
+      </c>
+      <c r="F65" t="s">
+        <v>187</v>
+      </c>
+      <c r="G65">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H65">
+        <v>212</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65" t="s">
+        <v>335</v>
+      </c>
+      <c r="K65" t="s">
+        <v>2</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" t="s">
+        <v>486</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" t="s">
+        <v>192</v>
+      </c>
+      <c r="E66" t="s">
+        <v>84</v>
+      </c>
+      <c r="F66" t="s">
+        <v>187</v>
+      </c>
+      <c r="G66">
+        <v>0.15</v>
+      </c>
+      <c r="H66">
+        <v>212</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66" t="s">
+        <v>335</v>
+      </c>
+      <c r="K66" t="s">
+        <v>2</v>
+      </c>
+      <c r="L66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" t="s">
+        <v>492</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" t="s">
+        <v>192</v>
+      </c>
+      <c r="E67" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" t="s">
+        <v>187</v>
+      </c>
+      <c r="G67">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="H67">
+        <v>212</v>
+      </c>
+      <c r="I67" t="s">
+        <v>19</v>
+      </c>
+      <c r="J67" t="s">
+        <v>335</v>
+      </c>
+      <c r="K67" t="s">
+        <v>2</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>490</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" t="s">
+        <v>192</v>
+      </c>
+      <c r="E68" t="s">
+        <v>86</v>
+      </c>
+      <c r="F68" t="s">
+        <v>187</v>
+      </c>
+      <c r="G68">
+        <v>0.155</v>
+      </c>
+      <c r="H68">
+        <v>212</v>
+      </c>
+      <c r="I68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" t="s">
+        <v>335</v>
+      </c>
+      <c r="K68" t="s">
+        <v>2</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>179</v>
+      </c>
+      <c r="B69" t="s">
+        <v>482</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D69" t="s">
+        <v>192</v>
+      </c>
+      <c r="E69" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" t="s">
+        <v>187</v>
+      </c>
+      <c r="G69">
+        <v>0.155</v>
+      </c>
+      <c r="H69">
+        <v>212</v>
+      </c>
+      <c r="I69" t="s">
+        <v>19</v>
+      </c>
+      <c r="J69" t="s">
+        <v>335</v>
+      </c>
+      <c r="K69" t="s">
+        <v>2</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" t="s">
+        <v>482</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D70" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" t="s">
+        <v>89</v>
+      </c>
+      <c r="F70" t="s">
+        <v>187</v>
+      </c>
+      <c r="G70">
+        <v>0.155</v>
+      </c>
+      <c r="H70">
+        <v>212</v>
+      </c>
+      <c r="I70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J70" t="s">
+        <v>335</v>
+      </c>
+      <c r="K70" t="s">
+        <v>2</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>179</v>
+      </c>
+      <c r="B71" t="s">
+        <v>482</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" t="s">
+        <v>192</v>
+      </c>
+      <c r="E71" t="s">
+        <v>90</v>
+      </c>
+      <c r="F71" t="s">
+        <v>187</v>
+      </c>
+      <c r="G71">
+        <v>0.155</v>
+      </c>
+      <c r="H71">
+        <v>212</v>
+      </c>
+      <c r="I71" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71" t="s">
+        <v>335</v>
+      </c>
+      <c r="K71" t="s">
+        <v>2</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" t="s">
+        <v>487</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D72" t="s">
+        <v>192</v>
+      </c>
+      <c r="E72" t="s">
+        <v>95</v>
+      </c>
+      <c r="F72" t="s">
+        <v>187</v>
+      </c>
+      <c r="G72">
+        <v>0.155</v>
+      </c>
+      <c r="H72">
+        <v>212</v>
+      </c>
+      <c r="I72" t="s">
+        <v>19</v>
+      </c>
+      <c r="J72" t="s">
+        <v>335</v>
+      </c>
+      <c r="K72" t="s">
+        <v>2</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" t="s">
+        <v>481</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D73" t="s">
+        <v>192</v>
+      </c>
+      <c r="E73" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" t="s">
+        <v>187</v>
+      </c>
+      <c r="G73">
+        <v>0.155</v>
+      </c>
+      <c r="H73">
+        <v>212</v>
+      </c>
+      <c r="I73" t="s">
+        <v>19</v>
+      </c>
+      <c r="J73" t="s">
+        <v>335</v>
+      </c>
+      <c r="K73" t="s">
+        <v>2</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" t="s">
+        <v>481</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D74" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" t="s">
+        <v>96</v>
+      </c>
+      <c r="F74" t="s">
+        <v>187</v>
+      </c>
+      <c r="G74">
+        <v>0.155</v>
+      </c>
+      <c r="H74">
+        <v>212</v>
+      </c>
+      <c r="I74" t="s">
+        <v>19</v>
+      </c>
+      <c r="J74" t="s">
+        <v>335</v>
+      </c>
+      <c r="K74" t="s">
+        <v>2</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" t="s">
+        <v>481</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D75" t="s">
+        <v>192</v>
+      </c>
+      <c r="E75" t="s">
+        <v>97</v>
+      </c>
+      <c r="F75" t="s">
+        <v>187</v>
+      </c>
+      <c r="G75">
+        <v>0.155</v>
+      </c>
+      <c r="H75">
+        <v>212</v>
+      </c>
+      <c r="I75" t="s">
+        <v>19</v>
+      </c>
+      <c r="J75" t="s">
+        <v>335</v>
+      </c>
+      <c r="K75" t="s">
+        <v>2</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" t="s">
+        <v>481</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D76" t="s">
+        <v>192</v>
+      </c>
+      <c r="E76" t="s">
+        <v>98</v>
+      </c>
+      <c r="F76" t="s">
+        <v>187</v>
+      </c>
+      <c r="G76">
+        <v>0.155</v>
+      </c>
+      <c r="H76">
+        <v>212</v>
+      </c>
+      <c r="I76" t="s">
+        <v>19</v>
+      </c>
+      <c r="J76" t="s">
+        <v>335</v>
+      </c>
+      <c r="K76" t="s">
+        <v>2</v>
+      </c>
+      <c r="L76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" t="s">
+        <v>481</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D77" t="s">
+        <v>192</v>
+      </c>
+      <c r="E77" t="s">
+        <v>99</v>
+      </c>
+      <c r="F77" t="s">
+        <v>187</v>
+      </c>
+      <c r="G77">
+        <v>0.155</v>
+      </c>
+      <c r="H77">
+        <v>212</v>
+      </c>
+      <c r="I77" t="s">
+        <v>19</v>
+      </c>
+      <c r="J77" t="s">
+        <v>335</v>
+      </c>
+      <c r="K77" t="s">
+        <v>2</v>
+      </c>
+      <c r="L77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" t="s">
+        <v>481</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D78" t="s">
+        <v>192</v>
+      </c>
+      <c r="E78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F78" t="s">
+        <v>187</v>
+      </c>
+      <c r="G78">
+        <v>0.155</v>
+      </c>
+      <c r="H78">
+        <v>212</v>
+      </c>
+      <c r="I78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J78" t="s">
+        <v>335</v>
+      </c>
+      <c r="K78" t="s">
+        <v>2</v>
+      </c>
+      <c r="L78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" t="s">
+        <v>481</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79" t="s">
+        <v>192</v>
+      </c>
+      <c r="E79" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" t="s">
+        <v>187</v>
+      </c>
+      <c r="G79">
+        <v>0.155</v>
+      </c>
+      <c r="H79">
+        <v>212</v>
+      </c>
+      <c r="I79" t="s">
+        <v>19</v>
+      </c>
+      <c r="J79" t="s">
+        <v>335</v>
+      </c>
+      <c r="K79" t="s">
+        <v>2</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>180</v>
+      </c>
+      <c r="B80" t="s">
+        <v>481</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D80" t="s">
+        <v>192</v>
+      </c>
+      <c r="E80" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" t="s">
+        <v>187</v>
+      </c>
+      <c r="G80">
+        <v>0.155</v>
+      </c>
+      <c r="H80">
+        <v>212</v>
+      </c>
+      <c r="I80" t="s">
+        <v>19</v>
+      </c>
+      <c r="J80" t="s">
+        <v>335</v>
+      </c>
+      <c r="K80" t="s">
+        <v>2</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" t="s">
+        <v>484</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" t="s">
+        <v>192</v>
+      </c>
+      <c r="E81" t="s">
+        <v>101</v>
+      </c>
+      <c r="F81" t="s">
+        <v>187</v>
+      </c>
+      <c r="G81">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="H81">
+        <v>212</v>
+      </c>
+      <c r="I81" t="s">
+        <v>19</v>
+      </c>
+      <c r="J81" t="s">
+        <v>335</v>
+      </c>
+      <c r="K81" t="s">
+        <v>2</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" t="s">
+        <v>491</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D82" t="s">
+        <v>192</v>
+      </c>
+      <c r="E82" t="s">
+        <v>102</v>
+      </c>
+      <c r="F82" t="s">
+        <v>187</v>
+      </c>
+      <c r="G82">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="H82">
+        <v>212</v>
+      </c>
+      <c r="I82" t="s">
+        <v>19</v>
+      </c>
+      <c r="J82" t="s">
+        <v>335</v>
+      </c>
+      <c r="K82" t="s">
+        <v>2</v>
+      </c>
+      <c r="L82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>176</v>
+      </c>
+      <c r="B83" t="s">
+        <v>485</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D83" t="s">
+        <v>192</v>
+      </c>
+      <c r="E83" t="s">
+        <v>100</v>
+      </c>
+      <c r="F83" t="s">
+        <v>187</v>
+      </c>
+      <c r="G83">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="H83">
+        <v>212</v>
+      </c>
+      <c r="I83" t="s">
+        <v>19</v>
+      </c>
+      <c r="J83" t="s">
+        <v>335</v>
+      </c>
+      <c r="K83" t="s">
+        <v>2</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" t="s">
+        <v>470</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D84" t="s">
+        <v>192</v>
+      </c>
+      <c r="E84" t="s">
+        <v>82</v>
+      </c>
+      <c r="F84" t="s">
+        <v>187</v>
+      </c>
+      <c r="G84">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H84">
+        <v>212</v>
+      </c>
+      <c r="I84" t="s">
+        <v>19</v>
+      </c>
+      <c r="J84" t="s">
+        <v>335</v>
+      </c>
+      <c r="K84" t="s">
+        <v>2</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" t="s">
+        <v>471</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" t="s">
+        <v>192</v>
+      </c>
+      <c r="E85" t="s">
+        <v>103</v>
+      </c>
+      <c r="F85" t="s">
+        <v>187</v>
+      </c>
+      <c r="G85">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H85">
+        <v>212</v>
+      </c>
+      <c r="I85" t="s">
+        <v>19</v>
+      </c>
+      <c r="J85" t="s">
+        <v>335</v>
+      </c>
+      <c r="K85" t="s">
+        <v>2</v>
+      </c>
+      <c r="L85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
+        <v>473</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D86" t="s">
+        <v>192</v>
+      </c>
+      <c r="E86" t="s">
+        <v>104</v>
+      </c>
+      <c r="F86" t="s">
+        <v>188</v>
+      </c>
+      <c r="G86">
+        <v>0.155</v>
+      </c>
+      <c r="H86">
+        <v>212</v>
+      </c>
+      <c r="I86" t="s">
+        <v>19</v>
+      </c>
+      <c r="J86" t="s">
+        <v>335</v>
+      </c>
+      <c r="K86" t="s">
+        <v>2</v>
+      </c>
+      <c r="L86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>483</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D87" t="s">
+        <v>192</v>
+      </c>
+      <c r="E87" t="s">
+        <v>189</v>
+      </c>
+      <c r="F87" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87">
+        <v>0.155</v>
+      </c>
+      <c r="H87">
+        <v>212</v>
+      </c>
+      <c r="I87" t="s">
+        <v>19</v>
+      </c>
+      <c r="J87" t="s">
+        <v>335</v>
+      </c>
+      <c r="K87" t="s">
+        <v>2</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L53" xr:uid="{B3B7B9A9-54CC-4D8F-A3E8-5153520FA509}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q4:R25">
-    <sortCondition ref="R4:R25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L54">
+    <sortCondition ref="H2:H54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6751,7 +8042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285A83FC-93DE-4924-85CE-252C66D09FA8}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>

</xml_diff>